<commit_message>
add custom widgets to example tempate
</commit_message>
<xml_diff>
--- a/forms/tables/exampleTable/forms/exampleTable/exampleTable.xlsx
+++ b/forms/tables/exampleTable/forms/exampleTable/exampleTable.xlsx
@@ -1,24 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Apps\CWBC\odk-precise-demo\app\config\tables\exampleTable\forms\exampleTable\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\apps\cwbc\cwbc-odkx-app\forms\tables\exampleTable\forms\exampleTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC8504B6-A5E9-412C-8679-0932C986EEE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{897FED95-9603-4C12-BA08-262A0933C007}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
     <sheet name="choices" sheetId="3" r:id="rId2"/>
     <sheet name="settings" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -27,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
   <si>
     <t>type</t>
   </si>
@@ -38,9 +46,6 @@
     <t>text</t>
   </si>
   <si>
-    <t>Enter your name</t>
-  </si>
-  <si>
     <t>yesno</t>
   </si>
   <si>
@@ -50,9 +55,6 @@
     <t>form_version</t>
   </si>
   <si>
-    <t>Example Form</t>
-  </si>
-  <si>
     <t>setting_name</t>
   </si>
   <si>
@@ -93,6 +95,39 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>clause</t>
+  </si>
+  <si>
+    <t>templatePath</t>
+  </si>
+  <si>
+    <t>begin screen</t>
+  </si>
+  <si>
+    <t>custom_date</t>
+  </si>
+  <si>
+    <t>Specify Date</t>
+  </si>
+  <si>
+    <t>../../../_templates/custom_date_picker.handlebars</t>
+  </si>
+  <si>
+    <t>custom_date_time</t>
+  </si>
+  <si>
+    <t>Specify Date &amp; Time</t>
+  </si>
+  <si>
+    <t>../../../_templates/custom_datetime_picker.handlebars</t>
+  </si>
+  <si>
+    <t>end screen</t>
+  </si>
+  <si>
+    <t>Templates Example Form</t>
   </si>
 </sst>
 </file>
@@ -537,38 +572,73 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>11</v>
-      </c>
       <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>3</v>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -590,95 +660,95 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.77734375" customWidth="1"/>
-    <col min="2" max="2" width="18.109375" customWidth="1"/>
-    <col min="3" max="3" width="23.44140625" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" ht="17.55" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" ht="17.55" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" ht="17.55" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" ht="17.55" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" ht="17.55" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:3" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="17" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="18" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -693,61 +763,61 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.44140625" customWidth="1"/>
-    <col min="2" max="2" width="24.109375" customWidth="1"/>
-    <col min="3" max="3" width="25.109375" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" customWidth="1"/>
+    <col min="3" max="3" width="25.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="B3" s="1">
         <v>20200307</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="14.55" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="14.65" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
update common template imports
</commit_message>
<xml_diff>
--- a/forms/tables/exampleTable/forms/exampleTable/exampleTable.xlsx
+++ b/forms/tables/exampleTable/forms/exampleTable/exampleTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\apps\cwbc\cwbc-odkx-app\forms\tables\exampleTable\forms\exampleTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B7EC1B2-27AF-4B19-B78D-ED688BDC6940}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{994EE08B-3BB7-41B1-8549-8A1F580D62F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7155" yWindow="2040" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
   <si>
     <t>type</t>
   </si>
@@ -124,10 +124,19 @@
     <t>Templates Example Form</t>
   </si>
   <si>
-    <t>../../../templates/custom_date_picker.handlebars</t>
-  </si>
-  <si>
-    <t>../../../templates/custom_datetime_picker.handlebars</t>
+    <t>../../../../assets/templates/custom_date_picker.handlebars</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>reusable templates are automatically copied to asset folder</t>
+  </si>
+  <si>
+    <t>custom_datetime_picker.handlebars</t>
+  </si>
+  <si>
+    <t>templates in same folder can be directly imported</t>
   </si>
 </sst>
 </file>
@@ -572,15 +581,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="7" max="7" width="26" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -599,8 +611,11 @@
       <c r="F1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>22</v>
       </c>
@@ -608,7 +623,7 @@
       <c r="C2" s="1"/>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>2</v>
       </c>
@@ -621,8 +636,11 @@
       <c r="F3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="G3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>2</v>
       </c>
@@ -633,10 +651,13 @@
         <v>26</v>
       </c>
       <c r="F4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+      <c r="G4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
fix change detection for custom date pickers
</commit_message>
<xml_diff>
--- a/forms/tables/exampleTable/forms/exampleTable/exampleTable.xlsx
+++ b/forms/tables/exampleTable/forms/exampleTable/exampleTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\apps\cwbc\cwbc-odkx-app\forms\tables\exampleTable\forms\exampleTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B87ABC7F-1AD0-4D57-9E48-3D334ECDC6A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8288B1C5-48A2-47F8-B9FD-A190EE7B883C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6420" yWindow="3045" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5505" yWindow="3300" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="256">
   <si>
     <t>type</t>
   </si>
@@ -722,18 +722,6 @@
     <t>prompt_type_name</t>
   </si>
   <si>
-    <t>select_one</t>
-  </si>
-  <si>
-    <t>Use native datalist element to provide select dropdown with text search</t>
-  </si>
-  <si>
-    <t>country_1</t>
-  </si>
-  <si>
-    <t>Select from list (autocomplete datalist)</t>
-  </si>
-  <si>
     <t>string</t>
   </si>
   <si>
@@ -804,9 +792,6 @@
   </si>
   <si>
     <t>../../../../assets/templates/custom_datetime_picker.handlebars</t>
-  </si>
-  <si>
-    <t>../../../../assets/templates/custom_select_autocomplete_datalist.handlebars</t>
   </si>
   <si>
     <t>Picker to populate date using calendar widget and button to specify 'now'</t>
@@ -1264,10 +1249,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1281,7 +1266,7 @@
         <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>0</v>
@@ -1302,10 +1287,10 @@
         <v>30</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -1331,7 +1316,7 @@
         <v>29</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="51" x14ac:dyDescent="0.2">
@@ -1345,74 +1330,74 @@
         <v>26</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="C5" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5" t="s">
-        <v>231</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>232</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>257</v>
-      </c>
+        <v>254</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>237</v>
+      </c>
+      <c r="B5" t="s">
+        <v>240</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="F5" s="5"/>
       <c r="H5" s="5" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="C6" s="5" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="51" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="D6" s="1"/>
+      <c r="F6" s="5" t="s">
         <v>241</v>
       </c>
-      <c r="B6" t="s">
-        <v>244</v>
-      </c>
-      <c r="D6" s="1"/>
-      <c r="F6" s="5"/>
       <c r="H6" s="5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+      <c r="C8" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="C7" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="D7" s="1"/>
-      <c r="F7" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+      <c r="F8" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="63.75" x14ac:dyDescent="0.2">
       <c r="C9" s="5" t="s">
         <v>249</v>
       </c>
       <c r="E9" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="H9" s="5" t="s">
         <v>250</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>260</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>251</v>
       </c>
       <c r="I9">
         <v>1</v>
@@ -1421,28 +1406,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="C10" s="5" t="s">
-        <v>253</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>252</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>254</v>
-      </c>
-      <c r="I10">
-        <v>1</v>
-      </c>
-      <c r="J10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1510,7 +1475,7 @@
         <v>31</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -1521,7 +1486,7 @@
         <v>31</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>33</v>
@@ -1532,7 +1497,7 @@
         <v>31</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>34</v>
@@ -3677,7 +3642,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3696,26 +3661,26 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="B3" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>249</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>253</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add text and integer inputs with do not know button
</commit_message>
<xml_diff>
--- a/forms/tables/exampleTable/forms/exampleTable/exampleTable.xlsx
+++ b/forms/tables/exampleTable/forms/exampleTable/exampleTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\apps\cwbc\cwbc-odkx-app\forms\tables\exampleTable\forms\exampleTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8066B653-CA85-4033-B4AC-E2C57A1BB954}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{591EE5EA-E14A-4051-933F-C594A8BEDF1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5505" yWindow="3300" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18090" yWindow="2745" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="269">
   <si>
     <t>type</t>
   </si>
@@ -816,13 +816,37 @@
   </si>
   <si>
     <t>Select a number from 1-5 (invalid choice will flag error on next)</t>
+  </si>
+  <si>
+    <t>number_3</t>
+  </si>
+  <si>
+    <t>Same as above, but with additional button for don't know</t>
+  </si>
+  <si>
+    <t>inputAttributes.showIDK</t>
+  </si>
+  <si>
+    <t>custom_text</t>
+  </si>
+  <si>
+    <t>text_1</t>
+  </si>
+  <si>
+    <t>Input text, or don't know (-99)</t>
+  </si>
+  <si>
+    <t>Same as above for text input</t>
+  </si>
+  <si>
+    <t>Input a number, or don't know (-99)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -854,6 +878,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -894,7 +925,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1264,10 +1295,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1276,7 +1307,7 @@
     <col min="8" max="8" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -1307,8 +1338,11 @@
       <c r="J1" s="5" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1" s="5" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>22</v>
       </c>
@@ -1317,9 +1351,9 @@
       <c r="D2" s="1"/>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:10" ht="51" x14ac:dyDescent="0.2">
-      <c r="C3" t="s">
-        <v>2</v>
+    <row r="3" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="C3" s="5" t="s">
+        <v>264</v>
       </c>
       <c r="E3" t="s">
         <v>23</v>
@@ -1334,7 +1368,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
         <v>2</v>
       </c>
@@ -1351,7 +1385,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="63.75" x14ac:dyDescent="0.2">
       <c r="C5" s="5" t="s">
         <v>229</v>
       </c>
@@ -1371,7 +1405,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>241</v>
       </c>
@@ -1384,7 +1418,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="63.75" x14ac:dyDescent="0.2">
       <c r="C7" s="5" t="s">
         <v>234</v>
       </c>
@@ -1396,12 +1430,12 @@
         <v>240</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="C9" s="5" t="s">
         <v>249</v>
       </c>
@@ -1421,7 +1455,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="63.75" x14ac:dyDescent="0.2">
       <c r="C10" s="5" t="s">
         <v>253</v>
       </c>
@@ -1441,8 +1475,42 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="11" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="C11" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="K11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="C12" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="K12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>27</v>
       </c>
     </row>
@@ -3674,10 +3742,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{769F93AD-2A70-4DD2-A169-0433B4A27062}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3718,8 +3786,17 @@
         <v>253</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>233</v>
+      </c>
+      <c r="B5" t="s">
+        <v>264</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
update example table comments
</commit_message>
<xml_diff>
--- a/forms/tables/exampleTable/forms/exampleTable/exampleTable.xlsx
+++ b/forms/tables/exampleTable/forms/exampleTable/exampleTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\apps\cwbc\cwbc-odkx-app\forms\tables\exampleTable\forms\exampleTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9CF390E-0CDC-41EC-ADE0-338686E31E70}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{697ADFD5-181B-487A-8AFD-812CB9716502}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9045" yWindow="3450" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5505" yWindow="3300" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -931,10 +931,10 @@
     <t>Section 2</t>
   </si>
   <si>
-    <t>Similar to user_branch type, displays a list of available sections, links, and additional completion taken from [branch_label]_complete variable in form</t>
-  </si>
-  <si>
     <t>Presents a checkbox to mark section as complete. Name should match branch name for tracking on custom_contents_page</t>
+  </si>
+  <si>
+    <t>Similar to user_branch type, displays a list of available sections, links, and additional completion taken from [branch_label]_complete variable in form. The list of sections should be defined in choices</t>
   </si>
 </sst>
 </file>
@@ -1478,7 +1478,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T964"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
@@ -1548,7 +1548,7 @@
       <c r="S2" s="7"/>
       <c r="T2" s="7"/>
     </row>
-    <row r="3" spans="1:20" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="17"/>
       <c r="C3" s="17"/>
@@ -1562,7 +1562,7 @@
         <v>292</v>
       </c>
       <c r="G3" s="23" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="H3" s="9"/>
       <c r="I3" s="9"/>
@@ -4984,8 +4984,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{248F424D-7B2D-41FA-9307-27C050305B00}">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5205,7 +5205,7 @@
         <v>293</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
update custom date pickers as custom prompt types
</commit_message>
<xml_diff>
--- a/forms/tables/exampleTable/forms/exampleTable/exampleTable.xlsx
+++ b/forms/tables/exampleTable/forms/exampleTable/exampleTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\apps\cwbc\cwbc-odkx-app\forms\tables\exampleTable\forms\exampleTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{697ADFD5-181B-487A-8AFD-812CB9716502}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B028B8F4-3585-44FF-8278-328B4B25303B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5505" yWindow="3300" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="299">
   <si>
     <t>type</t>
   </si>
@@ -43,9 +43,6 @@
     <t>name</t>
   </si>
   <si>
-    <t>text</t>
-  </si>
-  <si>
     <t>yesno</t>
   </si>
   <si>
@@ -124,9 +121,6 @@
     <t>Templates Example Form</t>
   </si>
   <si>
-    <t>../../../../assets/templates/custom_date_picker.handlebars</t>
-  </si>
-  <si>
     <t>comment</t>
   </si>
   <si>
@@ -805,9 +799,6 @@
     <t>Select a number from 1-5 (invalid will display warning only)</t>
   </si>
   <si>
-    <t>../../../../assets/templates/custom_datetime_picker.handlebars</t>
-  </si>
-  <si>
     <t>../../../../assets/templates/custom_select_autocomplete_datalist.handlebars</t>
   </si>
   <si>
@@ -935,6 +926,12 @@
   </si>
   <si>
     <t>Similar to user_branch type, displays a list of available sections, links, and additional completion taken from [branch_label]_complete variable in form. The list of sections should be defined in choices</t>
+  </si>
+  <si>
+    <t>custom_date_picker</t>
+  </si>
+  <si>
+    <t>custom_datetime_picker</t>
   </si>
 </sst>
 </file>
@@ -1478,8 +1475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T964"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1490,25 +1487,25 @@
   <sheetData>
     <row r="1" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G1" s="22" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="H1" s="10"/>
       <c r="I1" s="10"/>
@@ -1526,7 +1523,7 @@
     </row>
     <row r="2" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -1553,16 +1550,16 @@
       <c r="B3" s="17"/>
       <c r="C3" s="17"/>
       <c r="D3" s="18" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="F3" s="19" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="G3" s="23" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="H3" s="9"/>
       <c r="I3" s="9"/>
@@ -1581,7 +1578,7 @@
     <row r="4" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
       <c r="B4" s="20" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -1604,7 +1601,7 @@
     </row>
     <row r="5" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
@@ -1631,11 +1628,11 @@
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
       <c r="D6" s="7" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="E6" s="10"/>
       <c r="F6" s="20" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="G6" s="24"/>
       <c r="H6" s="10"/>
@@ -1655,7 +1652,7 @@
     <row r="7" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="7" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
@@ -1681,11 +1678,11 @@
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
       <c r="D8" s="7" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="E8" s="10"/>
       <c r="F8" s="20" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="G8" s="24"/>
       <c r="H8" s="10"/>
@@ -1705,7 +1702,7 @@
     <row r="9" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="20" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
@@ -1728,7 +1725,7 @@
     </row>
     <row r="10" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="B10" s="10"/>
       <c r="C10" s="10"/>
@@ -1755,11 +1752,11 @@
       <c r="B11" s="10"/>
       <c r="C11" s="10"/>
       <c r="D11" s="7" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="E11" s="10"/>
       <c r="F11" s="20" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="G11" s="24"/>
       <c r="H11" s="10"/>
@@ -1779,7 +1776,7 @@
     <row r="12" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="20" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
@@ -1805,11 +1802,11 @@
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
       <c r="D13" s="7" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="E13" s="10"/>
       <c r="F13" s="20" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="G13" s="24"/>
       <c r="H13" s="10"/>
@@ -1829,7 +1826,7 @@
     <row r="14" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="20" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
@@ -1852,7 +1849,7 @@
     </row>
     <row r="15" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
@@ -1879,11 +1876,11 @@
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
       <c r="D16" s="20" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="E16" s="10"/>
       <c r="F16" s="7" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="G16" s="24"/>
       <c r="H16" s="10"/>
@@ -1903,7 +1900,7 @@
     <row r="17" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="7" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
@@ -4984,8 +4981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{248F424D-7B2D-41FA-9307-27C050305B00}">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4996,42 +4993,42 @@
   <sheetData>
     <row r="1" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="13"/>
@@ -5039,102 +5036,98 @@
       <c r="E2" s="4"/>
       <c r="G2" s="14"/>
     </row>
-    <row r="3" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
       <c r="C3" s="5" t="s">
-        <v>264</v>
+        <v>297</v>
       </c>
       <c r="E3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" t="s">
         <v>23</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" s="5"/>
+      <c r="H3" s="5" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>298</v>
+      </c>
+      <c r="E4" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="51" x14ac:dyDescent="0.2">
-      <c r="C4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>25</v>
       </c>
-      <c r="F4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="5"/>
+      <c r="H4" s="5" t="s">
         <v>256</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="63.75" x14ac:dyDescent="0.2">
       <c r="C5" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" t="s">
         <v>229</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5" t="s">
-        <v>231</v>
-      </c>
       <c r="F5" s="5" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B6" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D6" s="1"/>
       <c r="F6" s="5"/>
       <c r="H6" s="5" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="63.75" x14ac:dyDescent="0.2">
       <c r="C7" s="5" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D7" s="1"/>
       <c r="F7" s="5" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="C9" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="H9" s="5" t="s">
         <v>249</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>250</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>260</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>251</v>
       </c>
       <c r="I9">
         <v>1</v>
@@ -5145,16 +5138,16 @@
     </row>
     <row r="10" spans="1:11" ht="63.75" x14ac:dyDescent="0.2">
       <c r="C10" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="H10" s="5" t="s">
         <v>252</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>254</v>
       </c>
       <c r="I10">
         <v>1</v>
@@ -5165,16 +5158,16 @@
     </row>
     <row r="11" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
       <c r="C11" s="5" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="K11" t="b">
         <v>1</v>
@@ -5182,16 +5175,16 @@
     </row>
     <row r="12" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C12" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="H12" s="5" t="s">
         <v>264</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>265</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>266</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>267</v>
       </c>
       <c r="K12" t="b">
         <v>1</v>
@@ -5199,18 +5192,18 @@
     </row>
     <row r="13" spans="1:11" s="11" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="C13" s="14" t="s">
+        <v>292</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>290</v>
+      </c>
+      <c r="H13" s="14" t="s">
         <v>295</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>293</v>
-      </c>
-      <c r="H13" s="14" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -5230,39 +5223,39 @@
   <sheetData>
     <row r="1" spans="1:10" s="11" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C1" s="13" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I1" s="15" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="J1" s="16" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="11" customFormat="1" ht="140.25" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="13"/>
@@ -5270,18 +5263,18 @@
       <c r="E2" s="4"/>
       <c r="G2" s="14"/>
       <c r="H2" s="11" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="I2" s="11" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="J2" s="14" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3" s="12"/>
       <c r="C3" s="13"/>
@@ -5312,2213 +5305,2213 @@
   <sheetData>
     <row r="1" spans="1:3" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" t="s">
-        <v>8</v>
-      </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="11" customFormat="1" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="3" spans="1:3" s="11" customFormat="1" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B16" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C16" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B17" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C17" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B20" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C20" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B21" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C21" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B22" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C22" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B23" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C23" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B24" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C24" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B25" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C25" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B26" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C26" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C27" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B28" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C28" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C29" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C30" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C31" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B32" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C32" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B33" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C33" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B34" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C34" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B35" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C35" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B36" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C36" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B37" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C37" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B38" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C38" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B39" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C39" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B40" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C40" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B41" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C41" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B42" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C42" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B43" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C43" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B44" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C44" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B45" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C45" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B46" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C46" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B47" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C47" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B48" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C48" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B49" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C49" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B50" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C50" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B51" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C51" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B52" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C52" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B53" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C53" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B54" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C54" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B55" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C55" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B56" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C56" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B57" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C57" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B58" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C58" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B59" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C59" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B60" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C60" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B61" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C61" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B62" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C62" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B63" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C63" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B64" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C64" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B65" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C65" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B66" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C66" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B67" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C67" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B68" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C68" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B69" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C69" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B70" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C70" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B71" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C71" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B72" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C72" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B73" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C73" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B74" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C74" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B75" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C75" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B76" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C76" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B77" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C77" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B78" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C78" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B79" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C79" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B80" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C80" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B81" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C81" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B82" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C82" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B83" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C83" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B84" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C84" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B85" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C85" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B86" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C86" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B87" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C87" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B88" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C88" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B89" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C89" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B90" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C90" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B91" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C91" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B92" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C92" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B93" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C93" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B94" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C94" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B95" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C95" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B96" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C96" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B97" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C97" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B98" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C98" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B99" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C99" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B100" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C100" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B101" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C101" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B102" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C102" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B103" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C103" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B104" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C104" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B105" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C105" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B106" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C106" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B107" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C107" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B108" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C108" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B109" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C109" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B110" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C110" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B111" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C111" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B112" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C112" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B113" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C113" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B114" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C114" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B115" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C115" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B116" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C116" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B117" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C117" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B118" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C118" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B119" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C119" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B120" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C120" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B121" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C121" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B122" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C122" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="123" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B123" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C123" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="124" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B124" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C124" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B125" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C125" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B126" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C126" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B127" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C127" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B128" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C128" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="129" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B129" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C129" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="130" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B130" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C130" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="131" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B131" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C131" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="132" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B132" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C132" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="133" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B133" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C133" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="134" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B134" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C134" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="135" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B135" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C135" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="136" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B136" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C136" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="137" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B137" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C137" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="138" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B138" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C138" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="139" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B139" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C139" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="140" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B140" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C140" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="141" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B141" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C141" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="142" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B142" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C142" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="143" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B143" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C143" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="144" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B144" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C144" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="145" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B145" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C145" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="146" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B146" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C146" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="147" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B147" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C147" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="148" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B148" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C148" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="149" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B149" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C149" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="150" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B150" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C150" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="151" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B151" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C151" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="152" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B152" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C152" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="153" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B153" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C153" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="154" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B154" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C154" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="155" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B155" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C155" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="156" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B156" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C156" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="157" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B157" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C157" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="158" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B158" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C158" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="159" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B159" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C159" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="160" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B160" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C160" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="161" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B161" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C161" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="162" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B162" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C162" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="163" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B163" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C163" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="164" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B164" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C164" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="165" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B165" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C165" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="166" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B166" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C166" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="167" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B167" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C167" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="168" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B168" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C168" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="169" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B169" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C169" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="170" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B170" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C170" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="171" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B171" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C171" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="172" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B172" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C172" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="173" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B173" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C173" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="174" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B174" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C174" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="175" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B175" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C175" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="176" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B176" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C176" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="177" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B177" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C177" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="178" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B178" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C178" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="179" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B179" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C179" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="180" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B180" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C180" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="181" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A181" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B181" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C181" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="182" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B182" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C182" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="183" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B183" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C183" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="184" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B184" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C184" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="185" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A185" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B185" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C185" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="186" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A186" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B186" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C186" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="187" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A187" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B187" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C187" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="188" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A188" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B188" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C188" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="189" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A189" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B189" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C189" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="190" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A190" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B190" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C190" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="191" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B191" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C191" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="192" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B192" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C192" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="193" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A193" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B193" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C193" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="194" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A194" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B194" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C194" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="195" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A195" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B195" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C195" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="196" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A196" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B196" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C196" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="197" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A197" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B197" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C197" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="198" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A198" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B198" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C198" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="199" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A199" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B199" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C199" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="200" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A200" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B200" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C200" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="201" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A201" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B201" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C201" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
   </sheetData>
@@ -7534,10 +7527,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{769F93AD-2A70-4DD2-A169-0433B4A27062}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7551,55 +7544,71 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B3" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B5" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>295</v>
+        <v>292</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>231</v>
+      </c>
+      <c r="B8" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>231</v>
+      </c>
+      <c r="B9" t="s">
+        <v>298</v>
       </c>
     </row>
   </sheetData>
@@ -7625,26 +7634,26 @@
   <sheetData>
     <row r="1" spans="1:3" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1">
         <v>20200308</v>
@@ -7652,18 +7661,18 @@
     </row>
     <row r="4" spans="1:3" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="14.65" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
add custom screen to fix scroll issues and example
</commit_message>
<xml_diff>
--- a/forms/tables/exampleTable/forms/exampleTable/exampleTable.xlsx
+++ b/forms/tables/exampleTable/forms/exampleTable/exampleTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\apps\cwbc\cwbc-odkx-app\forms\tables\exampleTable\forms\exampleTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B028B8F4-3585-44FF-8278-328B4B25303B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36E46118-50C1-400C-84CA-1C9C17DA42F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="743" uniqueCount="303">
   <si>
     <t>type</t>
   </si>
@@ -847,9 +847,6 @@
     <t>../config/assets/templates/custom_test_screen.handlebars</t>
   </si>
   <si>
-    <t>The custom screen will also contain information about any questions in the section</t>
-  </si>
-  <si>
     <t>branch_label</t>
   </si>
   <si>
@@ -932,6 +929,21 @@
   </si>
   <si>
     <t>custom_datetime_picker</t>
+  </si>
+  <si>
+    <t>custom_prompts_screen</t>
+  </si>
+  <si>
+    <t>custom_note_test</t>
+  </si>
+  <si>
+    <t>Example custom screen with template copied from examples</t>
+  </si>
+  <si>
+    <t>custom screen template, extends standard screen template so that all prompts are displayed in the same way as standard screen, with additional method to fix scroll position issue</t>
+  </si>
+  <si>
+    <t>This is a custom screen that has additonal render methods to fix a bug where sometimes the scroll position would not set correctly</t>
   </si>
 </sst>
 </file>
@@ -989,22 +1001,26 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1487,7 +1503,7 @@
   <sheetData>
     <row r="1" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>19</v>
@@ -1505,7 +1521,7 @@
         <v>11</v>
       </c>
       <c r="G1" s="22" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H1" s="10"/>
       <c r="I1" s="10"/>
@@ -1523,7 +1539,7 @@
     </row>
     <row r="2" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -1550,16 +1566,16 @@
       <c r="B3" s="17"/>
       <c r="C3" s="17"/>
       <c r="D3" s="18" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F3" s="19" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="G3" s="23" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="H3" s="9"/>
       <c r="I3" s="9"/>
@@ -1578,7 +1594,7 @@
     <row r="4" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
       <c r="B4" s="20" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -1601,7 +1617,7 @@
     </row>
     <row r="5" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
@@ -1628,11 +1644,11 @@
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
       <c r="D6" s="7" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E6" s="10"/>
       <c r="F6" s="20" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G6" s="24"/>
       <c r="H6" s="10"/>
@@ -1652,7 +1668,7 @@
     <row r="7" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
@@ -1678,11 +1694,11 @@
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
       <c r="D8" s="7" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E8" s="10"/>
       <c r="F8" s="20" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G8" s="24"/>
       <c r="H8" s="10"/>
@@ -1702,7 +1718,7 @@
     <row r="9" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="20" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
@@ -1725,7 +1741,7 @@
     </row>
     <row r="10" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B10" s="10"/>
       <c r="C10" s="10"/>
@@ -1752,11 +1768,11 @@
       <c r="B11" s="10"/>
       <c r="C11" s="10"/>
       <c r="D11" s="7" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E11" s="10"/>
       <c r="F11" s="20" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G11" s="24"/>
       <c r="H11" s="10"/>
@@ -1776,7 +1792,7 @@
     <row r="12" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="20" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
@@ -1802,11 +1818,11 @@
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
       <c r="D13" s="7" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E13" s="10"/>
       <c r="F13" s="20" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="G13" s="24"/>
       <c r="H13" s="10"/>
@@ -1826,7 +1842,7 @@
     <row r="14" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="20" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
@@ -1849,7 +1865,7 @@
     </row>
     <row r="15" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
@@ -1876,11 +1892,11 @@
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
       <c r="D16" s="20" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E16" s="10"/>
       <c r="F16" s="7" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G16" s="24"/>
       <c r="H16" s="10"/>
@@ -1900,7 +1916,7 @@
     <row r="17" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="7" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
@@ -4981,8 +4997,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{248F424D-7B2D-41FA-9307-27C050305B00}">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5038,7 +5054,7 @@
     </row>
     <row r="3" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
       <c r="C3" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E3" t="s">
         <v>22</v>
@@ -5053,7 +5069,7 @@
     </row>
     <row r="4" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E4" t="s">
         <v>24</v>
@@ -5192,13 +5208,13 @@
     </row>
     <row r="13" spans="1:11" s="11" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="C13" s="14" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
@@ -5213,13 +5229,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F37591D9-367F-4A0C-9E4B-E7990E14B855}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" customWidth="1"/>
+    <col min="6" max="6" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.7109375" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="39.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" s="11" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
@@ -5243,17 +5268,17 @@
       <c r="G1" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="15" t="s">
+        <v>266</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>268</v>
+      </c>
+      <c r="J1" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="15" t="s">
-        <v>266</v>
-      </c>
-      <c r="J1" s="16" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" s="11" customFormat="1" ht="140.25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:10" s="11" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>21</v>
       </c>
@@ -5263,13 +5288,13 @@
       <c r="E2" s="4"/>
       <c r="G2" s="14"/>
       <c r="H2" s="11" t="s">
-        <v>270</v>
-      </c>
-      <c r="I2" s="11" t="s">
         <v>267</v>
       </c>
+      <c r="I2" s="14" t="s">
+        <v>269</v>
+      </c>
       <c r="J2" s="14" t="s">
-        <v>269</v>
+        <v>300</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -5281,7 +5306,64 @@
       <c r="D3" s="12"/>
       <c r="E3" s="4"/>
       <c r="G3" s="14"/>
-      <c r="J3" s="14"/>
+      <c r="I3" s="14"/>
+    </row>
+    <row r="4" spans="1:10" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A4" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>298</v>
+      </c>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" s="11" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A5" s="12"/>
+      <c r="C5" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>299</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="11" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A6" s="12"/>
+      <c r="C6" s="14" t="s">
+        <v>251</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>250</v>
+      </c>
+      <c r="F6" s="14"/>
+    </row>
+    <row r="7" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="C7" s="14" t="s">
+        <v>251</v>
+      </c>
+      <c r="D7" s="11"/>
+      <c r="E7" s="14" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="C8" s="14" t="s">
+        <v>261</v>
+      </c>
+      <c r="D8" s="11"/>
+      <c r="E8" s="14" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="12" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5316,24 +5398,24 @@
     </row>
     <row r="2" spans="1:3" s="11" customFormat="1" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="B2" s="14" t="s">
         <v>281</v>
       </c>
-      <c r="B2" s="14" t="s">
-        <v>282</v>
-      </c>
       <c r="C2" s="14" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="3" spans="1:3" s="11" customFormat="1" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -7584,15 +7666,15 @@
         <v>233</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
+        <v>290</v>
+      </c>
+      <c r="B7" s="14" t="s">
         <v>291</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -7600,7 +7682,7 @@
         <v>231</v>
       </c>
       <c r="B8" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -7608,7 +7690,7 @@
         <v>231</v>
       </c>
       <c r="B9" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add profile screening page and summary table
</commit_message>
<xml_diff>
--- a/forms/tables/exampleTable/forms/exampleTable/exampleTable.xlsx
+++ b/forms/tables/exampleTable/forms/exampleTable/exampleTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\apps\cwbc\cwbc-odkx-app\forms\tables\exampleTable\forms\exampleTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36E46118-50C1-400C-84CA-1C9C17DA42F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F82131A-5710-46CD-8160-3F57136F3A24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5232,15 +5232,18 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
     <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
     <col min="5" max="5" width="18.85546875" customWidth="1"/>
-    <col min="6" max="6" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.140625" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" customWidth="1"/>
     <col min="8" max="8" width="31.7109375" customWidth="1"/>
     <col min="9" max="9" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="39.85546875" customWidth="1"/>

</xml_diff>